<commit_message>
Size check included for PropSI vector overload
Signed-off-by: Ian bell <ian.h.bell@gmail.com>
</commit_message>
<xml_diff>
--- a/wrappers/Excel/TestExcel.xlsx
+++ b/wrappers/Excel/TestExcel.xlsx
@@ -176,10 +176,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -256,7 +256,7 @@
                   <c:v>6.1220371526289217E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.021255884881164</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>83.914144952811796</c:v>
@@ -775,11 +775,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="137079040"/>
-        <c:axId val="137224576"/>
+        <c:axId val="141776000"/>
+        <c:axId val="141777920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="137079040"/>
+        <c:axId val="141776000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -807,12 +807,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137224576"/>
+        <c:crossAx val="141777920"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="137224576"/>
+        <c:axId val="141777920"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -841,7 +841,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137079040"/>
+        <c:crossAx val="141776000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -905,6 +905,7 @@
       <definedName name="CAS_code"/>
       <definedName name="Props"/>
       <definedName name="Props1"/>
+      <definedName name="PropsSI"/>
     </definedNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -1229,7 +1230,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,9 +1263,9 @@
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4" t="e">
         <f>[1]!Props1("R410A","Tcrit")</f>
-        <v>344.49400000000003</v>
+        <v>#VALUE!</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -1274,9 +1275,9 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4" t="e">
         <f>[1]!Props1("Propane","rhocrit")</f>
-        <v>220.47810000000001</v>
+        <v>#VALUE!</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -1286,9 +1287,9 @@
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="5">
-        <f>[1]!Props("D","T",298.15,"P",101.325,"Air")</f>
-        <v>1.1843184838675069</v>
+      <c r="B8" s="4">
+        <f>[1]!PropsSI("Dmolar","T",298.15,"P",101325,"REFPROP::Nitrogen")</f>
+        <v>40.881921595106235</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -1298,9 +1299,9 @@
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5">
-        <f>[1]!Props("T","P",101.325,"Q",0,"Water")-273.15</f>
-        <v>99.974295847683209</v>
+      <c r="B9" s="4">
+        <f>[1]!PropsSI("T","P",101325,"Q",0,"REFPROP::Water")-273.15</f>
+        <v>99.974295847697647</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
@@ -1310,8 +1311,8 @@
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="5">
-        <f>[1]!Props("T","P",101.325,"Q",0,"REFPROP-Water")-273.15</f>
+      <c r="B10" s="4">
+        <f>[1]!PropsSI("T","P",101325,"Q",0,"REFPROP::Water")-273.15</f>
         <v>99.974295847697647</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1325,27 +1326,27 @@
       <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="5" t="str">
+      <c r="B11" s="4" t="e">
         <f>[1]!CAS_code("Water")</f>
-        <v>7732-18-5</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="5" t="str">
+      <c r="B12" s="4" t="e">
         <f>[1]!Props1("A","B")</f>
-        <v>CoolProp error: Fluid "A" is an invalid fluid</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="5">
-        <f>[1]!Props("V","T",300,"P",101.325,"EG-20%")</f>
-        <v>1.3814217810500947E-3</v>
+      <c r="B13" s="4" t="e">
+        <f>[1]!Props("V","T",300,"P",101.325,"BRINE::EG[20%]")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
@@ -1362,8 +1363,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,13 +1374,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1490,9 +1491,9 @@
         <f>[2]!Props("D","T",B7,"Q",1,"Water")</f>
         <v>9.4070520080230726E-3</v>
       </c>
-      <c r="F7">
-        <f>[2]!Props("H","T",B7,"Q",0,"Water")</f>
-        <v>42.021255884881164</v>
+      <c r="F7" t="e">
+        <f>[1]!Props("H","T",B7,"Q",0,"Water")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="G7">
         <f>[2]!Props("H","T",B7,"Q",1,"Water")</f>

</xml_diff>

<commit_message>
Build architecture is working; wrappers building for EES, C#, Java, all the shared libraries
Signed-off-by: Ian bell <ian.h.bell@gmail.com>
</commit_message>
<xml_diff>
--- a/wrappers/Excel/TestExcel.xlsx
+++ b/wrappers/Excel/TestExcel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Critical temperature of R410A:</t>
   </si>
@@ -104,9 +104,6 @@
     <t>kJ/kg</t>
   </si>
   <si>
-    <t>(but calling REFPROP)</t>
-  </si>
-  <si>
     <t>b) Install the CoolProp Add-in</t>
   </si>
   <si>
@@ -123,6 +120,12 @@
   </si>
   <si>
     <t>Brine viscosity:</t>
+  </si>
+  <si>
+    <t>COOLPROP</t>
+  </si>
+  <si>
+    <t>Expected value</t>
   </si>
 </sst>
 </file>
@@ -775,11 +778,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="141776000"/>
-        <c:axId val="141777920"/>
+        <c:axId val="228716928"/>
+        <c:axId val="228718848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="141776000"/>
+        <c:axId val="228716928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -807,12 +810,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141777920"/>
+        <c:crossAx val="228718848"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141777920"/>
+        <c:axId val="228718848"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -841,7 +844,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141776000"/>
+        <c:crossAx val="228716928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -902,9 +905,8 @@
       <sheetName val="Sheet3"/>
     </sheetNames>
     <definedNames>
-      <definedName name="CAS_code"/>
       <definedName name="Props"/>
-      <definedName name="Props1"/>
+      <definedName name="Props1SI"/>
       <definedName name="PropsSI"/>
     </definedNames>
     <sheetDataSet>
@@ -1230,13 +1232,14 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1251,105 +1254,110 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="4" t="e">
-        <f>[1]!Props1("R410A","Tcrit")</f>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="e">
+        <f>[1]!Props1SI("R410A","Tcrit")</f>
         <v>#VALUE!</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4" t="e">
-        <f>[1]!Props1("Propane","rhocrit")</f>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4" t="e">
+        <f>[1]!Props1SI("Propane","rhocrit")</f>
         <v>#VALUE!</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="4">
-        <f>[1]!PropsSI("Dmolar","T",298.15,"P",101325,"REFPROP::Nitrogen")</f>
-        <v>40.881921595106235</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" t="s">
         <v>3</v>
+      </c>
+      <c r="C8" s="4">
+        <f>[1]!PropsSI("Dmass","T",298.15,"P",101325,"HEOS::Nitrogen")</f>
+        <v>1.1452448929366679</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="4">
-        <f>[1]!PropsSI("T","P",101325,"Q",0,"REFPROP::Water")-273.15</f>
-        <v>99.974295847697647</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C9" s="4" t="e">
+        <f>[1]!PropsSI("T","P",101325,"Q",0,"HEOS::Water")-273.15</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4">
         <f>[1]!PropsSI("T","P",101325,"Q",0,"REFPROP::Water")-273.15</f>
         <v>99.974295847697647</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="4" t="e">
-        <f>[1]!CAS_code("Water")</f>
+        <v>21</v>
+      </c>
+      <c r="C11" s="4" t="e">
+        <f>[1]!Props1SI("Water","CAS")</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="4" t="e">
-        <f>[1]!Props1("A","B")</f>
+        <v>22</v>
+      </c>
+      <c r="C12" s="4" t="e">
+        <f>[1]!Props1SI("A","B")</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="4" t="e">
-        <f>[1]!Props("V","T",300,"P",101.325,"BRINE::EG[20%]")</f>
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="4" t="e">
+        <f>[1]!PropsSI("V","T",300,"P",101.325,"BRINE::EG[20%]")</f>
         <v>#VALUE!</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>